<commit_message>
fix(spreads): Fixed logic for determining end of picks
</commit_message>
<xml_diff>
--- a/content/_data/NFL 2022 week 12.xlsx
+++ b/content/_data/NFL 2022 week 12.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="122">
   <si>
     <t xml:space="preserve">                               SPREAD POOL 2022</t>
   </si>
@@ -54,172 +54,175 @@
     <t>AARON</t>
   </si>
   <si>
+    <t>** WEEK # 12**</t>
+  </si>
+  <si>
+    <t>BUFF</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
     <t>buff  -9 1/2  DET</t>
   </si>
   <si>
-    <t>BUFF</t>
-  </si>
-  <si>
-    <t>DET</t>
+    <t>NYG</t>
+  </si>
+  <si>
+    <t>BOYS</t>
   </si>
   <si>
     <t>BOYS  -9 1/2  nyg</t>
   </si>
   <si>
-    <t>NYG</t>
-  </si>
-  <si>
-    <t>BOYS</t>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>N.E.</t>
+  </si>
+  <si>
+    <t>MIN**</t>
   </si>
   <si>
     <t>MIN  -2 1/2  n.e.</t>
   </si>
   <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>N.E.</t>
-  </si>
-  <si>
-    <t>MIN**</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
+    <t>BALT</t>
+  </si>
+  <si>
+    <t>BALT**</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
     <t>balt  -3 1/2  JAX</t>
   </si>
   <si>
-    <t>BALT</t>
-  </si>
-  <si>
-    <t>BALT**</t>
-  </si>
-  <si>
-    <t>JAX</t>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>CAR</t>
   </si>
   <si>
     <t>den  -1 1/2  CAR</t>
   </si>
   <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>CAR</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WASH</t>
+  </si>
+  <si>
+    <t>ATL</t>
   </si>
   <si>
     <t>WASH  -4 1/2  atl</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>WASH</t>
-  </si>
-  <si>
-    <t>ATL</t>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>NYJ</t>
   </si>
   <si>
     <t>nyj  -5 1/2  CHI</t>
   </si>
   <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>NYJ</t>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>TEN**</t>
+  </si>
+  <si>
+    <t>CIN</t>
   </si>
   <si>
     <t>cin  -2 1/2  TEN</t>
   </si>
   <si>
-    <t>TEN</t>
-  </si>
-  <si>
-    <t>TEN**</t>
-  </si>
-  <si>
-    <t>CIN</t>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>HOU</t>
   </si>
   <si>
     <t>MIA  -13 1/2  hou</t>
   </si>
   <si>
-    <t>MIA</t>
-  </si>
-  <si>
-    <t>HOU</t>
+    <t>T.B.**</t>
+  </si>
+  <si>
+    <t>T.B.</t>
+  </si>
+  <si>
+    <t>CLEV</t>
   </si>
   <si>
     <t>t.b.  -3 1/2  CLEV</t>
   </si>
   <si>
-    <t>T.B.**</t>
-  </si>
-  <si>
-    <t>T.B.</t>
-  </si>
-  <si>
-    <t>CLEV</t>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>ARZ</t>
   </si>
   <si>
     <t>lac  -2 1/2  ARZ</t>
   </si>
   <si>
-    <t>LAC</t>
-  </si>
-  <si>
-    <t>ARZ</t>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>LVR</t>
   </si>
   <si>
     <t>SEA  -3 1/2  lvr</t>
   </si>
   <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>LVR</t>
+    <t>S.F.</t>
+  </si>
+  <si>
+    <t>N.O.</t>
   </si>
   <si>
     <t>S.F.  -9 1/2  n.o.</t>
   </si>
   <si>
-    <t>S.F.</t>
-  </si>
-  <si>
-    <t>N.O.</t>
+    <t>K.C.</t>
+  </si>
+  <si>
+    <t>RAMS</t>
   </si>
   <si>
     <t>K.C.  -15 1/2  rams</t>
   </si>
   <si>
-    <t>K.C.</t>
-  </si>
-  <si>
-    <t>RAMS</t>
+    <t>PHIL</t>
+  </si>
+  <si>
+    <t>PHIL**</t>
+  </si>
+  <si>
+    <t>G.B.</t>
   </si>
   <si>
     <t>PHIL  -6 1/2  g.b.</t>
   </si>
   <si>
-    <t>PHIL</t>
-  </si>
-  <si>
-    <t>PHIL**</t>
-  </si>
-  <si>
-    <t>G.B.</t>
+    <t>INDY</t>
+  </si>
+  <si>
+    <t>PITT</t>
+  </si>
+  <si>
+    <t>PITT**</t>
   </si>
   <si>
     <t>INDY  -2 1/2  pitt</t>
-  </si>
-  <si>
-    <t>INDY</t>
-  </si>
-  <si>
-    <t>PITT</t>
-  </si>
-  <si>
-    <t>PITT**</t>
   </si>
   <si>
     <t xml:space="preserve">41    </t>
@@ -400,13 +403,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="20"/>
@@ -422,7 +431,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -823,234 +832,237 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="11" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="14" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="15" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="21" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="14" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="21" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1373,30 +1385,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="77" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="77" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="77" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="79" width="0.8621428571428571" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="78" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="79" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="78" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="79" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="78" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="80" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="79" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="80" width="0.8621428571428571" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="79" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="80" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="79" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="80" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="81" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="34.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1421,7 +1433,7 @@
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="24">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="24.75">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1453,15 +1465,11 @@
         <v>10</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="14">
-        <v>28</v>
-      </c>
+      <c r="L2" s="14"/>
       <c r="M2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="16">
-        <v>25</v>
-      </c>
+      <c r="N2" s="16"/>
       <c r="O2" s="17"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1509,7 +1517,7 @@
         <v>14</v>
       </c>
       <c r="N3" s="23">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="8"/>
@@ -1551,11 +1559,15 @@
         <v>15</v>
       </c>
       <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
+      <c r="L4" s="21">
+        <v>28</v>
+      </c>
       <c r="M4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="23"/>
+      <c r="N4" s="23">
+        <v>20</v>
+      </c>
       <c r="O4" s="7"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -1597,7 +1609,7 @@
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="21"/>
-      <c r="M5" s="26" t="s">
+      <c r="M5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="N5" s="23"/>
@@ -1622,7 +1634,7 @@
       <c r="J6" s="18"/>
       <c r="K6" s="20"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="26" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="23"/>
@@ -1939,7 +1951,9 @@
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
+      <c r="M13" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="N13" s="27"/>
       <c r="O13" s="17"/>
       <c r="P13" s="8"/>
@@ -1962,8 +1976,8 @@
       <c r="J14" s="18"/>
       <c r="K14" s="20"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="22" t="s">
-        <v>47</v>
+      <c r="M14" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="17"/>
@@ -2142,7 +2156,9 @@
       </c>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="22"/>
+      <c r="M18" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="N18" s="23"/>
       <c r="O18" s="17"/>
       <c r="P18" s="8"/>
@@ -2152,7 +2168,7 @@
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="23.25">
       <c r="A19" s="29"/>
       <c r="B19" s="18"/>
       <c r="C19" s="29"/>
@@ -2165,8 +2181,8 @@
       <c r="J19" s="29"/>
       <c r="K19" s="20"/>
       <c r="L19" s="21"/>
-      <c r="M19" s="22" t="s">
-        <v>59</v>
+      <c r="M19" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="N19" s="23"/>
       <c r="O19" s="17"/>
@@ -2177,7 +2193,7 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="23.25">
       <c r="A20" s="18" t="s">
         <v>60</v>
       </c>
@@ -2210,7 +2226,9 @@
       </c>
       <c r="K20" s="20"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="22"/>
+      <c r="M20" s="22" t="s">
+        <v>63</v>
+      </c>
       <c r="N20" s="27"/>
       <c r="O20" s="17"/>
       <c r="P20" s="8"/>
@@ -2220,7 +2238,7 @@
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="23.25">
       <c r="A21" s="31"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
@@ -2233,8 +2251,8 @@
       <c r="J21" s="31"/>
       <c r="K21" s="20"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="22" t="s">
-        <v>63</v>
+      <c r="M21" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="N21" s="23"/>
       <c r="O21" s="17"/>
@@ -2278,7 +2296,9 @@
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
+      <c r="M22" s="22" t="s">
+        <v>67</v>
+      </c>
       <c r="N22" s="27"/>
       <c r="O22" s="17"/>
       <c r="P22" s="8"/>
@@ -2302,8 +2322,8 @@
       <c r="K23" s="20"/>
       <c r="L23" s="21"/>
       <c r="M23" s="22"/>
-      <c r="N23" s="23" t="s">
-        <v>30</v>
+      <c r="N23" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="O23" s="17"/>
       <c r="P23" s="8"/>
@@ -2314,40 +2334,42 @@
       <c r="U23" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="24.95">
-      <c r="A24" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="B24" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="C24" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="E24" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="F24" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="34" t="s">
+      <c r="G24" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="40"/>
+      <c r="H24" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24" s="38"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="41" t="s">
+        <v>30</v>
+      </c>
       <c r="O24" s="17"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -2359,20 +2381,20 @@
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="24.95">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="N25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="N25" s="43"/>
       <c r="O25" s="17"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
@@ -2383,42 +2405,42 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="24.95">
       <c r="A26" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="46" t="s">
         <v>81</v>
       </c>
+      <c r="G26" s="47" t="s">
+        <v>82</v>
+      </c>
       <c r="H26" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K26" s="20"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="N26" s="49" t="s">
+      <c r="L26" s="48"/>
+      <c r="M26" s="49" t="s">
         <v>86</v>
+      </c>
+      <c r="N26" s="50" t="s">
+        <v>87</v>
       </c>
       <c r="O26" s="17"/>
       <c r="P26" s="8"/>
@@ -2445,28 +2467,28 @@
         <v>12</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J27" s="18" t="s">
         <v>13</v>
       </c>
       <c r="K27" s="20"/>
-      <c r="L27" s="50">
+      <c r="L27" s="51">
         <v>1</v>
       </c>
-      <c r="M27" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="N27" s="52">
+      <c r="M27" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="N27" s="53">
         <v>102</v>
       </c>
       <c r="O27" s="17"/>
@@ -2509,13 +2531,13 @@
         <v>16</v>
       </c>
       <c r="K28" s="20"/>
-      <c r="L28" s="53">
+      <c r="L28" s="54">
         <v>2</v>
       </c>
-      <c r="M28" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="N28" s="52">
+      <c r="M28" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="N28" s="53">
         <v>96</v>
       </c>
       <c r="O28" s="17"/>
@@ -2557,14 +2579,14 @@
       <c r="J29" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="55"/>
-      <c r="L29" s="53">
+      <c r="K29" s="56"/>
+      <c r="L29" s="54">
         <v>2</v>
       </c>
-      <c r="M29" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="N29" s="56">
+      <c r="M29" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="N29" s="57">
         <v>96</v>
       </c>
       <c r="O29" s="17"/>
@@ -2587,13 +2609,13 @@
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="20"/>
-      <c r="L30" s="53">
+      <c r="L30" s="54">
         <v>4</v>
       </c>
-      <c r="M30" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="N30" s="56">
+      <c r="M30" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="N30" s="57">
         <v>95</v>
       </c>
       <c r="O30" s="17"/>
@@ -2636,13 +2658,13 @@
         <v>25</v>
       </c>
       <c r="K31" s="20"/>
-      <c r="L31" s="53">
+      <c r="L31" s="54">
         <v>5</v>
       </c>
-      <c r="M31" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="N31" s="52">
+      <c r="M31" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="N31" s="53">
         <v>92</v>
       </c>
       <c r="O31" s="17"/>
@@ -2685,13 +2707,13 @@
         <v>28</v>
       </c>
       <c r="K32" s="20"/>
-      <c r="L32" s="57">
+      <c r="L32" s="58">
         <v>5</v>
       </c>
-      <c r="M32" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="N32" s="58">
+      <c r="M32" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="N32" s="59">
         <v>92</v>
       </c>
       <c r="O32" s="17"/>
@@ -2734,13 +2756,13 @@
         <v>31</v>
       </c>
       <c r="K33" s="20"/>
-      <c r="L33" s="53">
+      <c r="L33" s="54">
         <v>7</v>
       </c>
-      <c r="M33" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="N33" s="56">
+      <c r="M33" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="N33" s="57">
         <v>91</v>
       </c>
       <c r="O33" s="17"/>
@@ -2765,7 +2787,7 @@
         <v>35</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>34</v>
@@ -2774,7 +2796,7 @@
         <v>35</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>35</v>
@@ -2783,13 +2805,13 @@
         <v>34</v>
       </c>
       <c r="K34" s="20"/>
-      <c r="L34" s="57">
+      <c r="L34" s="58">
         <v>8</v>
       </c>
-      <c r="M34" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="N34" s="56">
+      <c r="M34" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="N34" s="57">
         <v>90</v>
       </c>
       <c r="O34" s="17"/>
@@ -2832,13 +2854,13 @@
         <v>37</v>
       </c>
       <c r="K35" s="20"/>
-      <c r="L35" s="53">
+      <c r="L35" s="54">
         <v>8</v>
       </c>
-      <c r="M35" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="N35" s="56">
+      <c r="M35" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="N35" s="57">
         <v>90</v>
       </c>
       <c r="O35" s="17"/>
@@ -2860,7 +2882,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>42</v>
@@ -2881,13 +2903,13 @@
         <v>41</v>
       </c>
       <c r="K36" s="20"/>
-      <c r="L36" s="57">
+      <c r="L36" s="58">
         <v>8</v>
       </c>
-      <c r="M36" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="N36" s="52">
+      <c r="M36" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="N36" s="53">
         <v>90</v>
       </c>
       <c r="O36" s="17"/>
@@ -2930,13 +2952,13 @@
         <v>46</v>
       </c>
       <c r="K37" s="20"/>
-      <c r="L37" s="53">
+      <c r="L37" s="54">
         <v>8</v>
       </c>
-      <c r="M37" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="N37" s="56">
+      <c r="M37" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="N37" s="57">
         <v>90</v>
       </c>
       <c r="O37" s="17"/>
@@ -2959,13 +2981,13 @@
       <c r="I38" s="24"/>
       <c r="J38" s="18"/>
       <c r="K38" s="20"/>
-      <c r="L38" s="57">
+      <c r="L38" s="58">
         <v>8</v>
       </c>
-      <c r="M38" s="54" t="s">
+      <c r="M38" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="N38" s="52">
+      <c r="N38" s="53">
         <v>90</v>
       </c>
       <c r="O38" s="17"/>
@@ -3008,13 +3030,13 @@
         <v>49</v>
       </c>
       <c r="K39" s="20"/>
-      <c r="L39" s="53">
+      <c r="L39" s="54">
         <v>13</v>
       </c>
-      <c r="M39" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="N39" s="56">
+      <c r="M39" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="N39" s="57">
         <v>89</v>
       </c>
       <c r="O39" s="17"/>
@@ -3033,7 +3055,7 @@
         <v>51</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>51</v>
@@ -3056,14 +3078,14 @@
       <c r="J40" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="K40" s="59"/>
-      <c r="L40" s="57">
+      <c r="K40" s="60"/>
+      <c r="L40" s="58">
         <v>13</v>
       </c>
-      <c r="M40" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="N40" s="60">
+      <c r="M40" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="N40" s="61">
         <v>89</v>
       </c>
       <c r="O40" s="17"/>
@@ -3079,7 +3101,7 @@
         <v>54</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>54</v>
@@ -3106,13 +3128,13 @@
         <v>54</v>
       </c>
       <c r="K41" s="20"/>
-      <c r="L41" s="53">
+      <c r="L41" s="54">
         <v>13</v>
       </c>
-      <c r="M41" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="N41" s="52">
+      <c r="M41" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="N41" s="53">
         <v>89</v>
       </c>
       <c r="O41" s="17"/>
@@ -3154,14 +3176,14 @@
       <c r="J42" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="61"/>
-      <c r="L42" s="53">
+      <c r="K42" s="62"/>
+      <c r="L42" s="54">
         <v>13</v>
       </c>
-      <c r="M42" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="N42" s="52">
+      <c r="M42" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="N42" s="53">
         <v>89</v>
       </c>
       <c r="O42" s="17"/>
@@ -3184,13 +3206,13 @@
       <c r="I43" s="24"/>
       <c r="J43" s="18"/>
       <c r="K43" s="20"/>
-      <c r="L43" s="53">
+      <c r="L43" s="54">
         <v>17</v>
       </c>
-      <c r="M43" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="N43" s="52">
+      <c r="M43" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="N43" s="53">
         <v>85</v>
       </c>
       <c r="O43" s="17"/>
@@ -3211,7 +3233,7 @@
       <c r="C44" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="64" t="s">
+      <c r="D44" s="65" t="s">
         <v>60</v>
       </c>
       <c r="E44" s="18" t="s">
@@ -3232,14 +3254,14 @@
       <c r="J44" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="K44" s="37"/>
-      <c r="L44" s="57">
+      <c r="K44" s="38"/>
+      <c r="L44" s="58">
         <v>18</v>
       </c>
-      <c r="M44" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="N44" s="56">
+      <c r="M44" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="N44" s="57">
         <v>84</v>
       </c>
       <c r="O44" s="17"/>
@@ -3251,24 +3273,24 @@
       <c r="U44" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="24.95">
-      <c r="A45" s="65"/>
-      <c r="B45" s="65"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="18"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="65"/>
+      <c r="G45" s="66"/>
       <c r="H45" s="18"/>
       <c r="I45" s="24"/>
-      <c r="J45" s="65"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="53">
+      <c r="J45" s="66"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="54">
         <v>19</v>
       </c>
-      <c r="M45" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="N45" s="52">
+      <c r="M45" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="N45" s="53">
         <v>83</v>
       </c>
       <c r="O45" s="17"/>
@@ -3280,25 +3302,25 @@
       <c r="U45" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="24.95">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="65" t="s">
+      <c r="B46" s="66" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="65" t="s">
+      <c r="D46" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="65" t="s">
+      <c r="E46" s="66" t="s">
         <v>64</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G46" s="67" t="s">
+      <c r="G46" s="68" t="s">
         <v>64</v>
       </c>
       <c r="H46" s="18" t="s">
@@ -3307,17 +3329,17 @@
       <c r="I46" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J46" s="65" t="s">
+      <c r="J46" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="K46" s="37"/>
-      <c r="L46" s="53">
+      <c r="K46" s="38"/>
+      <c r="L46" s="54">
         <v>18</v>
       </c>
-      <c r="M46" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="N46" s="56">
+      <c r="M46" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="N46" s="57">
         <v>81</v>
       </c>
       <c r="O46" s="17"/>
@@ -3329,20 +3351,20 @@
       <c r="U46" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="24.95">
-      <c r="A47" s="68"/>
-      <c r="B47" s="69"/>
-      <c r="C47" s="68"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="69"/>
+      <c r="A47" s="69"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
       <c r="I47" s="18"/>
-      <c r="J47" s="68"/>
+      <c r="J47" s="69"/>
       <c r="K47" s="20"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="62"/>
-      <c r="N47" s="71"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="72"/>
       <c r="O47" s="17"/>
       <c r="P47" s="8"/>
       <c r="Q47" s="8"/>
@@ -3352,42 +3374,42 @@
       <c r="U47" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="24.95">
-      <c r="A48" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="34" t="s">
+      <c r="A48" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="B48" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="C48" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="D48" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="F48" s="34" t="s">
+      <c r="E48" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="G48" s="35" t="s">
+      <c r="F48" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="I48" s="34" t="s">
+      <c r="G48" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="J48" s="34" t="s">
+      <c r="H48" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="K48" s="72"/>
-      <c r="L48" s="53" t="s">
+      <c r="J48" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="K48" s="73"/>
+      <c r="L48" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="M48" s="62"/>
-      <c r="N48" s="73" t="s">
+      <c r="M48" s="63"/>
+      <c r="N48" s="74" t="s">
         <v>30</v>
       </c>
       <c r="O48" s="17"/>
@@ -3402,17 +3424,17 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="75"/>
-      <c r="L49" s="74"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="77"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="75"/>
       <c r="M49" s="7"/>
-      <c r="N49" s="74"/>
+      <c r="N49" s="75"/>
       <c r="O49" s="7"/>
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
@@ -3425,19 +3447,19 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="74"/>
+      <c r="L50" s="75"/>
       <c r="M50" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="N50" s="74"/>
+        <v>121</v>
+      </c>
+      <c r="N50" s="75"/>
       <c r="O50" s="7"/>
       <c r="P50" s="8"/>
       <c r="Q50" s="8"/>

</xml_diff>